<commit_message>
2017/11/6 穎驊 補 push
</commit_message>
<xml_diff>
--- a/AfterGratuationStatics/Resources/畢業生進路調查公務統計報表(學校分類).xlsx
+++ b/AfterGratuationStatics/Resources/畢業生進路調查公務統計報表(學校分類).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ED\Desktop\畢業生進路樣板(施工參考此)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ED\Documents\ischool_github\Counsel_SystemV2\AfterGratuationStatics\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2013,7 +2013,7 @@
   <dimension ref="A1:J300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2038,18 +2038,18 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="13" t="str">
-        <f>IFERROR(IF(FIND("國立",A2),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A2),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A2),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A2),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A2),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A2),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A2),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A2),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A2),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A2),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A2),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A2),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A2),"","A03私立大學校院日間部(含第二部、四技"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
+        <f>IFERROR(IF(FIND("國立",A2),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A2),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A2),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A2),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A2),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A2),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A2),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A2),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A2),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A2),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A2),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A2),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A2),"","A03私立大學校院日間部(含第二部、四技)"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B66" si="0">IFERROR(IF(FIND("國立",A3),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A3),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A3),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A3),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A3),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A3),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A3),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A3),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A3),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A3),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A3),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A3),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A3),"","A03私立大學校院日間部(含第二部、四技"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
+      <c r="B3" s="1" t="str">
+        <f t="shared" ref="B3:B66" si="0">IFERROR(IF(FIND("國立",A3),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A3),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A3),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A3),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A3),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A3),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A3),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A3),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A3),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A3),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A3),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A3),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A3),"","A03私立大學校院日間部(含第二部、四技)"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="str">
+      <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2064,7 +2064,7 @@
       <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="str">
+      <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2081,7 +2081,7 @@
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="str">
+      <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2098,7 +2098,7 @@
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="str">
+      <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2115,7 +2115,7 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="str">
+      <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2132,7 +2132,7 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="str">
+      <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="str">
+      <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2166,7 +2166,7 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="str">
+      <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2183,1735 +2183,1735 @@
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="str">
+      <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="str">
+      <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="str">
+      <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="str">
+      <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="str">
+      <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="str">
+      <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="str">
+      <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="str">
+      <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="str">
+      <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="str">
+      <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="str">
+      <c r="B22" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="str">
+      <c r="B23" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="str">
+      <c r="B24" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="str">
+      <c r="B25" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="str">
+      <c r="B26" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="str">
+      <c r="B27" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="str">
+      <c r="B28" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="str">
+      <c r="B29" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="str">
+      <c r="B30" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="str">
+      <c r="B31" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="str">
+      <c r="B32" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="str">
+      <c r="B33" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="str">
+      <c r="B34" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="str">
+      <c r="B35" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="str">
+      <c r="B36" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="str">
+      <c r="B37" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="str">
+      <c r="B38" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="str">
+      <c r="B39" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="str">
+      <c r="B40" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="str">
+      <c r="B41" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="str">
+      <c r="B42" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="str">
+      <c r="B43" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="str">
+      <c r="B44" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="str">
+      <c r="B45" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="str">
+      <c r="B46" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="str">
+      <c r="B47" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="str">
+      <c r="B48" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="str">
+      <c r="B49" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="str">
+      <c r="B50" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="str">
+      <c r="B51" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="str">
+      <c r="B52" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="str">
+      <c r="B53" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="str">
+      <c r="B54" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="str">
+      <c r="B55" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="str">
+      <c r="B56" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="str">
+      <c r="B57" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" t="str">
+      <c r="B58" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="str">
+      <c r="B59" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="str">
+      <c r="B60" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" t="str">
+      <c r="B61" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="str">
+      <c r="B62" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" t="str">
+      <c r="B63" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" t="str">
+      <c r="B64" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="str">
+      <c r="B65" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="str">
+      <c r="B66" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="str">
-        <f t="shared" ref="B67:B130" si="1">IFERROR(IF(FIND("國立",A67),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A67),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A67),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A67),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A67),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A67),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A67),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A67),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A67),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A67),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A67),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A67),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A67),"","A03私立大學校院日間部(含第二部、四技"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
+      <c r="B67" s="1" t="str">
+        <f t="shared" ref="B67:B130" si="1">IFERROR(IF(FIND("國立",A67),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A67),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A67),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A67),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A67),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A67),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A67),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A67),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A67),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A67),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A67),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A67),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A67),"","A03私立大學校院日間部(含第二部、四技)"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="str">
+      <c r="B68" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" t="str">
+      <c r="B69" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" t="str">
+      <c r="B70" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" t="str">
+      <c r="B71" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" t="str">
+      <c r="B72" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" t="str">
+      <c r="B73" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" t="str">
+      <c r="B74" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" t="str">
+      <c r="B75" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" t="str">
+      <c r="B76" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" t="str">
+      <c r="B77" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" t="str">
+      <c r="B78" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" t="str">
+      <c r="B79" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" t="str">
+      <c r="B80" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="str">
+      <c r="B81" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="str">
+      <c r="B82" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" t="str">
+      <c r="B83" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" t="str">
+      <c r="B84" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" t="str">
+      <c r="B85" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" t="str">
+      <c r="B86" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" t="str">
+      <c r="B87" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" t="str">
+      <c r="B88" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" t="str">
+      <c r="B89" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" t="str">
+      <c r="B90" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" t="str">
+      <c r="B91" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" t="str">
+      <c r="B92" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" t="str">
+      <c r="B93" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" t="str">
+      <c r="B94" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" t="str">
+      <c r="B95" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" t="str">
+      <c r="B96" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" t="str">
+      <c r="B97" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" t="str">
+      <c r="B98" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" t="str">
+      <c r="B99" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" t="str">
+      <c r="B100" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" t="str">
+      <c r="B101" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" t="str">
+      <c r="B102" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" t="str">
+      <c r="B103" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" t="str">
+      <c r="B104" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" t="str">
+      <c r="B105" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" t="str">
+      <c r="B106" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" t="str">
+      <c r="B107" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" t="str">
+      <c r="B108" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" t="str">
+      <c r="B109" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" t="str">
+      <c r="B110" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" t="str">
+      <c r="B111" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" t="str">
+      <c r="B112" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" t="str">
+      <c r="B113" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" t="str">
+      <c r="B114" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" t="str">
+      <c r="B115" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" t="str">
+      <c r="B116" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" t="str">
+      <c r="B117" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" t="str">
+      <c r="B118" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" t="str">
+      <c r="B119" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" t="str">
+      <c r="B120" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" t="str">
+      <c r="B121" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" t="str">
+      <c r="B122" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" t="str">
+      <c r="B123" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" t="str">
+      <c r="B124" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" t="str">
+      <c r="B125" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" t="str">
+      <c r="B126" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" t="str">
+      <c r="B127" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" t="str">
+      <c r="B128" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" t="str">
+      <c r="B129" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" t="str">
+      <c r="B130" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" t="str">
-        <f t="shared" ref="B131:B194" si="2">IFERROR(IF(FIND("國立",A131),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A131),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A131),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A131),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A131),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A131),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A131),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A131),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A131),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A131),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A131),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A131),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A131),"","A03私立大學校院日間部(含第二部、四技"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
+      <c r="B131" s="1" t="str">
+        <f t="shared" ref="B131:B194" si="2">IFERROR(IF(FIND("國立",A131),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A131),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A131),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A131),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A131),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A131),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A131),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A131),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A131),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A131),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A131),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A131),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A131),"","A03私立大學校院日間部(含第二部、四技)"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
         <v/>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" t="str">
+      <c r="B132" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" t="str">
+      <c r="B133" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" t="str">
+      <c r="B134" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" t="str">
+      <c r="B135" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" t="str">
+      <c r="B136" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" t="str">
+      <c r="B137" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" t="str">
+      <c r="B138" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" t="str">
+      <c r="B139" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" t="str">
+      <c r="B140" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" t="str">
+      <c r="B141" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" t="str">
+      <c r="B142" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" t="str">
+      <c r="B143" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" t="str">
+      <c r="B144" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" t="str">
+      <c r="B145" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" t="str">
+      <c r="B146" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" t="str">
+      <c r="B147" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" t="str">
+      <c r="B148" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" t="str">
+      <c r="B149" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" t="str">
+      <c r="B150" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" t="str">
+      <c r="B151" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" t="str">
+      <c r="B152" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" t="str">
+      <c r="B153" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" t="str">
+      <c r="B154" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" t="str">
+      <c r="B155" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" t="str">
+      <c r="B156" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" t="str">
+      <c r="B157" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" t="str">
+      <c r="B158" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" t="str">
+      <c r="B159" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" t="str">
+      <c r="B160" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" t="str">
+      <c r="B161" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" t="str">
+      <c r="B162" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" t="str">
+      <c r="B163" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" t="str">
+      <c r="B164" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165" t="str">
+      <c r="B165" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166" t="str">
+      <c r="B166" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167" t="str">
+      <c r="B167" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" t="str">
+      <c r="B168" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" t="str">
+      <c r="B169" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B170" t="str">
+      <c r="B170" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" t="str">
+      <c r="B171" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172" t="str">
+      <c r="B172" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173" t="str">
+      <c r="B173" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174" t="str">
+      <c r="B174" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175" t="str">
+      <c r="B175" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B176" t="str">
+      <c r="B176" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" t="str">
+      <c r="B177" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" t="str">
+      <c r="B178" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B179" t="str">
+      <c r="B179" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" t="str">
+      <c r="B180" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" t="str">
+      <c r="B181" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" t="str">
+      <c r="B182" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183" t="str">
+      <c r="B183" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184" t="str">
+      <c r="B184" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B185" t="str">
+      <c r="B185" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186" t="str">
+      <c r="B186" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B187" t="str">
+      <c r="B187" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B188" t="str">
+      <c r="B188" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189" t="str">
+      <c r="B189" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B190" t="str">
+      <c r="B190" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B191" t="str">
+      <c r="B191" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B192" t="str">
+      <c r="B192" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B193" t="str">
+      <c r="B193" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B194" t="str">
+      <c r="B194" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B195" t="str">
-        <f t="shared" ref="B195:B258" si="3">IFERROR(IF(FIND("國立",A195),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A195),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A195),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A195),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A195),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A195),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A195),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A195),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A195),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A195),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A195),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A195),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A195),"","A03私立大學校院日間部(含第二部、四技"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
+      <c r="B195" s="1" t="str">
+        <f t="shared" ref="B195:B258" si="3">IFERROR(IF(FIND("國立",A195),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A195),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A195),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A195),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A195),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A195),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A195),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A195),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A195),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A195),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A195),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A195),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A195),"","A03私立大學校院日間部(含第二部、四技)"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
         <v/>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B196" t="str">
+      <c r="B196" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B197" t="str">
+      <c r="B197" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B198" t="str">
+      <c r="B198" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B199" t="str">
+      <c r="B199" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B200" t="str">
+      <c r="B200" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B201" t="str">
+      <c r="B201" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B202" t="str">
+      <c r="B202" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B203" t="str">
+      <c r="B203" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B204" t="str">
+      <c r="B204" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B205" t="str">
+      <c r="B205" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B206" t="str">
+      <c r="B206" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B207" t="str">
+      <c r="B207" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B208" t="str">
+      <c r="B208" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B209" t="str">
+      <c r="B209" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B210" t="str">
+      <c r="B210" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B211" t="str">
+      <c r="B211" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B212" t="str">
+      <c r="B212" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B213" t="str">
+      <c r="B213" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B214" t="str">
+      <c r="B214" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B215" t="str">
+      <c r="B215" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B216" t="str">
+      <c r="B216" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B217" t="str">
+      <c r="B217" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B218" t="str">
+      <c r="B218" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B219" t="str">
+      <c r="B219" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B220" t="str">
+      <c r="B220" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B221" t="str">
+      <c r="B221" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B222" t="str">
+      <c r="B222" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B223" t="str">
+      <c r="B223" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B224" t="str">
+      <c r="B224" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B225" t="str">
+      <c r="B225" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B226" t="str">
+      <c r="B226" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B227" t="str">
+      <c r="B227" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B228" t="str">
+      <c r="B228" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B229" t="str">
+      <c r="B229" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B230" t="str">
+      <c r="B230" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B231" t="str">
+      <c r="B231" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B232" t="str">
+      <c r="B232" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B233" t="str">
+      <c r="B233" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B234" t="str">
+      <c r="B234" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B235" t="str">
+      <c r="B235" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B236" t="str">
+      <c r="B236" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B237" t="str">
+      <c r="B237" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B238" t="str">
+      <c r="B238" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B239" t="str">
+      <c r="B239" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B240" t="str">
+      <c r="B240" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B241" t="str">
+      <c r="B241" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B242" t="str">
+      <c r="B242" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B243" t="str">
+      <c r="B243" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B244" t="str">
+      <c r="B244" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B245" t="str">
+      <c r="B245" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B246" t="str">
+      <c r="B246" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B247" t="str">
+      <c r="B247" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B248" t="str">
+      <c r="B248" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B249" t="str">
+      <c r="B249" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B250" t="str">
+      <c r="B250" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B251" t="str">
+      <c r="B251" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B252" t="str">
+      <c r="B252" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B253" t="str">
+      <c r="B253" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B254" t="str">
+      <c r="B254" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B255" t="str">
+      <c r="B255" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B256" t="str">
+      <c r="B256" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B257" t="str">
+      <c r="B257" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="258" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B258" t="str">
+      <c r="B258" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="259" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B259" t="str">
-        <f t="shared" ref="B259:B300" si="4">IFERROR(IF(FIND("國立",A259),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A259),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A259),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A259),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A259),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A259),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A259),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A259),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A259),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A259),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A259),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A259),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A259),"","A03私立大學校院日間部(含第二部、四技"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
+      <c r="B259" s="1" t="str">
+        <f t="shared" ref="B259:B300" si="4">IFERROR(IF(FIND("國立",A259),"A01公立大學校院日間部(含第二部、四技)",),IFERROR(IF(FIND("臺灣警察專科學校",A259),"A10警察專科學校",),IFERROR(IF(FIND("國防大學",A259),"A11軍事院校",),IFERROR(IF(FIND("國防醫學院",A259),"A11軍事院校",),IFERROR(IF(FIND("中央警察大學",A259),"A09警察大學",),IFERROR(IF(FIND("陸軍專科學校",A259),"A11軍事院校",),IFERROR(IF(FIND("中華民國陸軍軍官學校",A259),"A11軍事院校",),IFERROR(IF(FIND("海軍軍官學校",A259),"A11軍事院校",),IFERROR(IF(FIND("中華民國空軍軍官學校",A259),"A11軍事院校",),IFERROR(IF(FIND("國立臺南護理專科學校",A259),"A05公立二專日間部",),IFERROR(IF(FIND("國立臺東專科學校",A259),"A05公立二專日間部",),IFERROR(IF(FIND("專科學校",A259),"A07私立二專日間部",),IFERROR(IF(ISBLANK(A259),"","A03私立大學校院日間部(含第二部、四技)"),"A03私立大學校院日間部(含第二部、四技)")))))))))))))</f>
         <v/>
       </c>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B260" t="str">
+      <c r="B260" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="261" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B261" t="str">
+      <c r="B261" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="262" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B262" t="str">
+      <c r="B262" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B263" t="str">
+      <c r="B263" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="264" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B264" t="str">
+      <c r="B264" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="265" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B265" t="str">
+      <c r="B265" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B266" t="str">
+      <c r="B266" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="267" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B267" t="str">
+      <c r="B267" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B268" t="str">
+      <c r="B268" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B269" t="str">
+      <c r="B269" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B270" t="str">
+      <c r="B270" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="271" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B271" t="str">
+      <c r="B271" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B272" t="str">
+      <c r="B272" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B273" t="str">
+      <c r="B273" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B274" t="str">
+      <c r="B274" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B275" t="str">
+      <c r="B275" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B276" t="str">
+      <c r="B276" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="277" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B277" t="str">
+      <c r="B277" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B278" t="str">
+      <c r="B278" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="279" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B279" t="str">
+      <c r="B279" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B280" t="str">
+      <c r="B280" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B281" t="str">
+      <c r="B281" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="282" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B282" t="str">
+      <c r="B282" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="283" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B283" t="str">
+      <c r="B283" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="284" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B284" t="str">
+      <c r="B284" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="285" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B285" t="str">
+      <c r="B285" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="286" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B286" t="str">
+      <c r="B286" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="287" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B287" t="str">
+      <c r="B287" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="288" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B288" t="str">
+      <c r="B288" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="289" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B289" t="str">
+      <c r="B289" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="290" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B290" t="str">
+      <c r="B290" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="291" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B291" t="str">
+      <c r="B291" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="292" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B292" t="str">
+      <c r="B292" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="293" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B293" t="str">
+      <c r="B293" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="294" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B294" t="str">
+      <c r="B294" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="295" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B295" t="str">
+      <c r="B295" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="296" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B296" t="str">
+      <c r="B296" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="297" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B297" t="str">
+      <c r="B297" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="298" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B298" t="str">
+      <c r="B298" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="299" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B299" t="str">
+      <c r="B299" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="300" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B300" t="str">
+      <c r="B300" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>

</xml_diff>